<commit_message>
perbaikan update plot penilai pegawai
</commit_message>
<xml_diff>
--- a/storage/dupak.xlsx
+++ b/storage/dupak.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="180">
   <si>
     <t xml:space="preserve">LAMPIRAN </t>
   </si>
@@ -49,7 +49,7 @@
     <t>NOMOR: B-xxx/BPS/02610/xx/xxxx</t>
   </si>
   <si>
-    <t>Masa Penilaian Tanggal: 01 Desember 2019 s/d 31 Desember 2019</t>
+    <t>Masa Penilaian Tanggal: 01 Januari 2019 s/d 31 Desember 2019</t>
   </si>
   <si>
     <t>I. KETERANGAN PERORANGAN</t>
@@ -61,25 +61,25 @@
     <t>:</t>
   </si>
   <si>
-    <t>Easbi Ikhsan, S.Tr.Stat, M.Stat</t>
+    <t>Ir. ERYA AFRIANUS</t>
   </si>
   <si>
     <t>NIP</t>
   </si>
   <si>
-    <t>199602192019012001</t>
+    <t>196704141994021001</t>
   </si>
   <si>
     <t>Nomor Seri Karpeg</t>
   </si>
   <si>
-    <t>A-3210</t>
+    <t>xxx</t>
   </si>
   <si>
     <t>Tempat dan Tanggal Lahir</t>
   </si>
   <si>
-    <t>Bangkok, 18 Februari 1996</t>
+    <t xml:space="preserve">xxx, </t>
   </si>
   <si>
     <t>Jenis Kelamin</t>
@@ -97,13 +97,13 @@
     <t>Pangkat/Golongan/TMT</t>
   </si>
   <si>
-    <t>Penata Muda - III/A/ 18 Februari 1996</t>
+    <t xml:space="preserve">Penata Muda - III/A/ </t>
   </si>
   <si>
     <t>Jabatan/TMT</t>
   </si>
   <si>
-    <t>Widyaiswara Ahli Muda/ 18 Februari 1996</t>
+    <t xml:space="preserve">Widyaiswara Ahli Muda/ </t>
   </si>
   <si>
     <t>Unit Kerja saat ini</t>
@@ -551,9 +551,6 @@
   </si>
   <si>
     <t>Jakarta, xx xx xxxx</t>
-  </si>
-  <si>
-    <t>xxx</t>
   </si>
   <si>
     <t>NIP. Xxx</t>
@@ -7432,7 +7429,7 @@
       <c r="N122" s="37"/>
       <c r="O122" s="37"/>
       <c r="P122" s="243" t="s">
-        <v>164</v>
+        <v>18</v>
       </c>
       <c r="Q122" s="243"/>
       <c r="R122" s="243"/>
@@ -7461,7 +7458,7 @@
       <c r="N123" s="104"/>
       <c r="O123" s="104"/>
       <c r="P123" s="239" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q123" s="239"/>
       <c r="R123" s="239"/>
@@ -7501,7 +7498,7 @@
     </row>
     <row r="125" spans="1:94" customHeight="1" ht="24.9" s="98" customFormat="1">
       <c r="B125" s="240" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C125" s="241"/>
       <c r="D125" s="241"/>
@@ -7530,7 +7527,7 @@
     <row r="126" spans="1:94" customHeight="1" ht="24.9" s="37" customFormat="1">
       <c r="B126" s="81"/>
       <c r="C126" s="82" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D126" s="83"/>
       <c r="E126" s="83"/>
@@ -7558,7 +7555,7 @@
       <c r="A127" s="96"/>
       <c r="B127" s="87"/>
       <c r="C127" s="88" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D127" s="89"/>
       <c r="E127" s="89"/>
@@ -7587,7 +7584,7 @@
       <c r="A128" s="41"/>
       <c r="B128" s="87"/>
       <c r="C128" s="91" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D128" s="92"/>
       <c r="E128" s="92"/>
@@ -7615,7 +7612,7 @@
       <c r="A129" s="41"/>
       <c r="B129" s="87"/>
       <c r="C129" s="91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D129" s="92"/>
       <c r="E129" s="92"/>
@@ -7653,7 +7650,7 @@
       <c r="L130" s="92"/>
       <c r="M130" s="90"/>
       <c r="O130" s="246" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P130" s="246"/>
       <c r="Q130" s="246"/>
@@ -7679,7 +7676,7 @@
       <c r="L131" s="92"/>
       <c r="M131" s="90"/>
       <c r="O131" s="247" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P131" s="247"/>
       <c r="Q131" s="247"/>
@@ -7727,7 +7724,7 @@
       <c r="J133" s="92"/>
       <c r="M133" s="90"/>
       <c r="O133" s="243" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P133" s="247"/>
       <c r="Q133" s="247"/>
@@ -7754,7 +7751,7 @@
       <c r="M134" s="103"/>
       <c r="N134" s="104"/>
       <c r="O134" s="239" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P134" s="239"/>
       <c r="Q134" s="239"/>
@@ -7839,7 +7836,7 @@
     <row r="138" spans="1:94" customHeight="1" ht="24.9" s="27" customFormat="1">
       <c r="A138" s="7"/>
       <c r="B138" s="240" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C138" s="241"/>
       <c r="D138" s="241"/>
@@ -7869,7 +7866,7 @@
       <c r="A139" s="7"/>
       <c r="B139" s="81"/>
       <c r="C139" s="82" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D139" s="83"/>
       <c r="E139" s="83"/>
@@ -7898,7 +7895,7 @@
       <c r="A140" s="7"/>
       <c r="B140" s="87"/>
       <c r="C140" s="88" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D140" s="89"/>
       <c r="E140" s="89"/>
@@ -7913,7 +7910,7 @@
       <c r="N140" s="89"/>
       <c r="O140" s="89"/>
       <c r="P140" s="89" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q140" s="89"/>
       <c r="R140" s="89"/>
@@ -7929,7 +7926,7 @@
       <c r="A141" s="93"/>
       <c r="B141" s="87"/>
       <c r="C141" s="91" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D141" s="92"/>
       <c r="E141" s="92"/>
@@ -7958,7 +7955,7 @@
       <c r="A142" s="41"/>
       <c r="B142" s="87"/>
       <c r="C142" s="91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D142" s="92"/>
       <c r="E142" s="92"/>
@@ -8023,7 +8020,7 @@
       <c r="L144" s="92"/>
       <c r="M144" s="90"/>
       <c r="P144" s="243" t="s">
-        <v>164</v>
+        <v>18</v>
       </c>
       <c r="Q144" s="243"/>
       <c r="R144" s="243"/>
@@ -8050,7 +8047,7 @@
       <c r="L145" s="92"/>
       <c r="M145" s="90"/>
       <c r="P145" s="246" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q145" s="246"/>
       <c r="R145" s="246"/>
@@ -8143,7 +8140,7 @@
       <c r="N149" s="37"/>
       <c r="O149" s="37"/>
       <c r="P149" s="243" t="s">
-        <v>164</v>
+        <v>18</v>
       </c>
       <c r="Q149" s="243"/>
       <c r="R149" s="243"/>
@@ -8166,7 +8163,7 @@
       <c r="N150" s="104"/>
       <c r="O150" s="104"/>
       <c r="P150" s="239" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q150" s="239"/>
       <c r="R150" s="239"/>
@@ -8196,7 +8193,7 @@
     </row>
     <row r="152" spans="1:94" customHeight="1" ht="24.9">
       <c r="B152" s="240" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C152" s="241"/>
       <c r="D152" s="241"/>
@@ -8220,7 +8217,7 @@
     <row r="153" spans="1:94" customHeight="1" ht="24.9">
       <c r="B153" s="81"/>
       <c r="C153" s="82" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D153" s="83"/>
       <c r="E153" s="83"/>
@@ -8243,7 +8240,7 @@
     <row r="154" spans="1:94" customHeight="1" ht="24.9">
       <c r="B154" s="87"/>
       <c r="C154" s="88" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D154" s="89"/>
       <c r="E154" s="89"/>
@@ -8258,7 +8255,7 @@
       <c r="N154" s="89"/>
       <c r="O154" s="89"/>
       <c r="P154" s="89" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q154" s="89"/>
       <c r="R154" s="89"/>
@@ -8268,7 +8265,7 @@
     <row r="155" spans="1:94" customHeight="1" ht="24.9">
       <c r="B155" s="87"/>
       <c r="C155" s="91" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D155" s="92"/>
       <c r="E155" s="92"/>
@@ -8291,7 +8288,7 @@
     <row r="156" spans="1:94" customHeight="1" ht="24.9" s="37" customFormat="1">
       <c r="B156" s="87"/>
       <c r="C156" s="91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D156" s="92"/>
       <c r="E156" s="92"/>
@@ -8331,7 +8328,7 @@
       <c r="N157" s="92"/>
       <c r="O157" s="92"/>
       <c r="P157" s="92" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q157" s="92"/>
       <c r="R157" s="92"/>
@@ -8383,7 +8380,7 @@
       <c r="N159" s="92"/>
       <c r="O159" s="92"/>
       <c r="P159" s="101" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q159" s="101"/>
       <c r="R159" s="101"/>
@@ -8410,7 +8407,7 @@
       <c r="N160" s="101"/>
       <c r="O160" s="101"/>
       <c r="P160" s="101" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q160" s="101"/>
       <c r="R160" s="101"/>

</xml_diff>

<commit_message>
sekretariat ->melihat detail per unsur dupak yg berbeda nilai.. dikasih warna mrah utnuk yg berbeda
</commit_message>
<xml_diff>
--- a/storage/dupak.xlsx
+++ b/storage/dupak.xlsx
@@ -49,7 +49,7 @@
     <t>NOMOR: B-xxx/BPS/02610/xx/xxxx</t>
   </si>
   <si>
-    <t>Masa Penilaian Tanggal: 01 January 2020 s/d 31 January 2020</t>
+    <t>Masa Penilaian Tanggal: 01 Februari 2020 s/d 21 Februari 2020</t>
   </si>
   <si>
     <t>I. KETERANGAN PERORANGAN</t>
@@ -61,13 +61,13 @@
     <t>:</t>
   </si>
   <si>
-    <t>MUHAMMAD KADDAFI SUYATNO SST</t>
+    <t>MOHAMMAD IRKHAM S.Si</t>
   </si>
   <si>
     <t>NIP</t>
   </si>
   <si>
-    <t>7</t>
+    <t>196810191991021001</t>
   </si>
   <si>
     <t>Nomor Seri Karpeg</t>
@@ -3585,7 +3585,7 @@
         <v>4</v>
       </c>
       <c r="M36" s="42">
-        <v>0.4</v>
+        <v>0.4.0</v>
       </c>
       <c r="N36" s="142"/>
       <c r="O36" s="142"/>
@@ -3615,7 +3615,7 @@
         <v>5</v>
       </c>
       <c r="M37" s="42">
-        <v>0.4</v>
+        <v>0.4.0</v>
       </c>
       <c r="N37" s="142"/>
       <c r="O37" s="142"/>
@@ -3645,7 +3645,7 @@
         <v>6</v>
       </c>
       <c r="M38" s="42">
-        <v>0.4</v>
+        <v>0.4.0</v>
       </c>
       <c r="N38" s="142"/>
       <c r="O38" s="142"/>
@@ -3675,7 +3675,7 @@
         <v>7</v>
       </c>
       <c r="M39" s="33">
-        <v>0.4</v>
+        <v>0.4.0</v>
       </c>
       <c r="N39" s="33"/>
       <c r="O39" s="33"/>
@@ -3729,7 +3729,7 @@
         <v>8</v>
       </c>
       <c r="M41" s="33">
-        <v>0.2</v>
+        <v>0.2.0</v>
       </c>
       <c r="N41" s="33"/>
       <c r="O41" s="33"/>
@@ -3764,7 +3764,7 @@
         <v>9</v>
       </c>
       <c r="M42" s="33">
-        <v>0.2</v>
+        <v>0.2.0</v>
       </c>
       <c r="N42" s="33"/>
       <c r="O42" s="33"/>
@@ -3799,7 +3799,7 @@
         <v>10</v>
       </c>
       <c r="M43" s="33">
-        <v>0.4</v>
+        <v>0.4.0</v>
       </c>
       <c r="N43" s="33"/>
       <c r="O43" s="33"/>
@@ -3837,7 +3837,7 @@
         <v>11</v>
       </c>
       <c r="M44" s="53">
-        <v>0.02</v>
+        <v>0.02.0</v>
       </c>
       <c r="N44" s="33"/>
       <c r="O44" s="33"/>
@@ -3849,7 +3849,7 @@
       <c r="U44" s="54"/>
       <c r="Z44" s="164"/>
       <c r="AE44" s="41">
-        <v>13.4</v>
+        <v>13.4.0</v>
       </c>
     </row>
     <row r="45" spans="1:94" customHeight="1" ht="24.9">
@@ -3868,7 +3868,7 @@
         <v>12</v>
       </c>
       <c r="M45" s="53">
-        <v>0.04</v>
+        <v>0.04.0</v>
       </c>
       <c r="N45" s="33"/>
       <c r="O45" s="33"/>
@@ -3880,7 +3880,7 @@
       <c r="U45" s="54"/>
       <c r="Z45" s="164"/>
       <c r="AE45" s="41">
-        <v>9.4</v>
+        <v>9.4.0</v>
       </c>
     </row>
     <row r="46" spans="1:94" customHeight="1" ht="24.9">
@@ -3899,7 +3899,7 @@
         <v>13</v>
       </c>
       <c r="M46" s="53">
-        <v>0.06</v>
+        <v>0.06.0</v>
       </c>
       <c r="N46" s="33"/>
       <c r="O46" s="33"/>
@@ -3927,7 +3927,7 @@
         <v>14</v>
       </c>
       <c r="M47" s="53">
-        <v>0.08</v>
+        <v>0.08.0</v>
       </c>
       <c r="N47" s="33"/>
       <c r="O47" s="33"/>
@@ -3956,7 +3956,7 @@
         <v>15</v>
       </c>
       <c r="M48" s="53">
-        <v>0.02</v>
+        <v>0.02.0</v>
       </c>
       <c r="N48" s="33"/>
       <c r="O48" s="33"/>
@@ -3984,7 +3984,7 @@
         <v>16</v>
       </c>
       <c r="M49" s="33">
-        <v>0.03</v>
+        <v>0.03.0</v>
       </c>
       <c r="N49" s="33"/>
       <c r="O49" s="33"/>
@@ -4011,7 +4011,7 @@
         <v>17</v>
       </c>
       <c r="M50" s="33">
-        <v>0.5</v>
+        <v>0.5.0</v>
       </c>
       <c r="N50" s="129"/>
       <c r="O50" s="129"/>
@@ -4038,7 +4038,7 @@
         <v>18</v>
       </c>
       <c r="M51" s="53">
-        <v>0.5</v>
+        <v>0.5.0</v>
       </c>
       <c r="N51" s="129"/>
       <c r="O51" s="33"/>
@@ -4090,7 +4090,7 @@
         <v>19</v>
       </c>
       <c r="M53" s="33">
-        <v>0.15</v>
+        <v>0.15.0</v>
       </c>
       <c r="N53" s="33"/>
       <c r="O53" s="33"/>
@@ -4124,7 +4124,7 @@
         <v>20</v>
       </c>
       <c r="M54" s="33">
-        <v>0.15</v>
+        <v>0.15.0</v>
       </c>
       <c r="N54" s="129"/>
       <c r="O54" s="33"/>
@@ -4158,7 +4158,7 @@
         <v>21</v>
       </c>
       <c r="M55" s="33">
-        <v>0.3</v>
+        <v>0.3.0</v>
       </c>
       <c r="N55" s="129"/>
       <c r="O55" s="33"/>
@@ -4270,7 +4270,7 @@
         <v>23</v>
       </c>
       <c r="M58" s="42">
-        <v>0.4</v>
+        <v>0.4.0</v>
       </c>
       <c r="N58" s="140"/>
       <c r="O58" s="140"/>
@@ -4299,7 +4299,7 @@
         <v>24</v>
       </c>
       <c r="M59" s="42">
-        <v>0.15</v>
+        <v>0.15.0</v>
       </c>
       <c r="N59" s="142"/>
       <c r="O59" s="142"/>
@@ -4333,7 +4333,7 @@
         <v>25</v>
       </c>
       <c r="M60" s="53">
-        <v>2.5</v>
+        <v>2.5.0</v>
       </c>
       <c r="N60" s="129"/>
       <c r="O60" s="129"/>
@@ -4362,7 +4362,7 @@
         <v>26</v>
       </c>
       <c r="M61" s="33">
-        <v>1.5</v>
+        <v>1.5.0</v>
       </c>
       <c r="N61" s="129"/>
       <c r="O61" s="129"/>
@@ -4658,7 +4658,7 @@
         <v>32</v>
       </c>
       <c r="M71" s="42">
-        <v>2.5</v>
+        <v>2.5.0</v>
       </c>
       <c r="N71" s="142"/>
       <c r="O71" s="142"/>
@@ -4737,7 +4737,7 @@
         <v>34</v>
       </c>
       <c r="M74" s="33">
-        <v>2.5</v>
+        <v>2.5.0</v>
       </c>
       <c r="N74" s="129"/>
       <c r="O74" s="33"/>
@@ -4843,7 +4843,7 @@
         <v>37</v>
       </c>
       <c r="M78" s="33">
-        <v>2.5</v>
+        <v>2.5.0</v>
       </c>
       <c r="N78" s="129"/>
       <c r="O78" s="33"/>
@@ -4934,7 +4934,7 @@
         <v>40</v>
       </c>
       <c r="M81" s="53">
-        <v>0.5</v>
+        <v>0.5.0</v>
       </c>
       <c r="N81" s="129"/>
       <c r="O81" s="129"/>
@@ -5364,7 +5364,7 @@
       <c r="K90" s="261"/>
       <c r="L90" s="173"/>
       <c r="M90" s="72">
-        <v>0.75</v>
+        <v>0.75.0</v>
       </c>
       <c r="N90" s="33"/>
       <c r="O90" s="33"/>
@@ -5467,7 +5467,7 @@
       <c r="K91" s="264"/>
       <c r="L91" s="174"/>
       <c r="M91" s="153">
-        <v>0.25</v>
+        <v>0.25.0</v>
       </c>
       <c r="N91" s="33"/>
       <c r="O91" s="33"/>
@@ -5770,7 +5770,7 @@
       <c r="K94" s="261"/>
       <c r="L94" s="173"/>
       <c r="M94" s="72">
-        <v>1.5</v>
+        <v>1.5.0</v>
       </c>
       <c r="N94" s="33"/>
       <c r="O94" s="33"/>

</xml_diff>

<commit_message>
Perubahan v.1.5.13 perubahan dengan menambahkan dokumen spmt dan stmt disertai proses penyesuaian dokumen berkas
</commit_message>
<xml_diff>
--- a/storage/dupak.xlsx
+++ b/storage/dupak.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="181">
   <si>
     <t xml:space="preserve">LAMPIRAN </t>
   </si>
@@ -49,7 +49,7 @@
     <t>NOMOR: B-xxx/BPS/02610/xx/xxxx</t>
   </si>
   <si>
-    <t>Masa Penilaian Tanggal: 01 Januari 2019 s/d 31 Desember 2019</t>
+    <t>Masa Penilaian Tanggal: 01 January 2019 s/d 01 January 2020</t>
   </si>
   <si>
     <t>I. KETERANGAN PERORANGAN</t>
@@ -61,25 +61,25 @@
     <t>:</t>
   </si>
   <si>
-    <t>MOHAMMAD IRKHAM S.Si</t>
+    <t>Dr. AHMADRISWAN NASUTION S.Si MT</t>
   </si>
   <si>
     <t>NIP</t>
   </si>
   <si>
-    <t>196810191991021001</t>
+    <t>197301251994121001</t>
   </si>
   <si>
     <t>Nomor Seri Karpeg</t>
   </si>
   <si>
-    <t>xxx</t>
+    <t>G.268466</t>
   </si>
   <si>
     <t>Tempat dan Tanggal Lahir</t>
   </si>
   <si>
-    <t xml:space="preserve">xxx, </t>
+    <t>Padang Sidempuan, 25 January 1973</t>
   </si>
   <si>
     <t>Jenis Kelamin</t>
@@ -91,19 +91,19 @@
     <t>Pendidikan yang telah diperhitungkan angka kreditnya</t>
   </si>
   <si>
-    <t>S-2</t>
+    <t>S-3</t>
   </si>
   <si>
     <t>Pangkat/Golongan/TMT</t>
   </si>
   <si>
-    <t xml:space="preserve">Penata Muda - III/A/ </t>
+    <t>Pembina Tingkat I - IV/B/ 25 January 1973</t>
   </si>
   <si>
     <t>Jabatan/TMT</t>
   </si>
   <si>
-    <t xml:space="preserve">Widyaiswara Ahli Muda/ </t>
+    <t>Widyaiswara Ahli Madya/ 25 January 1973</t>
   </si>
   <si>
     <t>Unit Kerja saat ini</t>
@@ -551,6 +551,9 @@
   </si>
   <si>
     <t>Jakarta, xx xx xxxx</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
   <si>
     <t>NIP. Xxx</t>
@@ -3585,7 +3588,7 @@
         <v>4</v>
       </c>
       <c r="M36" s="42">
-        <v>0.4.0</v>
+        <v>0.4</v>
       </c>
       <c r="N36" s="142"/>
       <c r="O36" s="142"/>
@@ -3615,7 +3618,7 @@
         <v>5</v>
       </c>
       <c r="M37" s="42">
-        <v>0.4.0</v>
+        <v>0.4</v>
       </c>
       <c r="N37" s="142"/>
       <c r="O37" s="142"/>
@@ -3645,7 +3648,7 @@
         <v>6</v>
       </c>
       <c r="M38" s="42">
-        <v>0.4.0</v>
+        <v>0.4</v>
       </c>
       <c r="N38" s="142"/>
       <c r="O38" s="142"/>
@@ -3675,7 +3678,7 @@
         <v>7</v>
       </c>
       <c r="M39" s="33">
-        <v>0.4.0</v>
+        <v>0.4</v>
       </c>
       <c r="N39" s="33"/>
       <c r="O39" s="33"/>
@@ -3729,7 +3732,7 @@
         <v>8</v>
       </c>
       <c r="M41" s="33">
-        <v>0.2.0</v>
+        <v>0.2</v>
       </c>
       <c r="N41" s="33"/>
       <c r="O41" s="33"/>
@@ -3764,7 +3767,7 @@
         <v>9</v>
       </c>
       <c r="M42" s="33">
-        <v>0.2.0</v>
+        <v>0.2</v>
       </c>
       <c r="N42" s="33"/>
       <c r="O42" s="33"/>
@@ -3799,7 +3802,7 @@
         <v>10</v>
       </c>
       <c r="M43" s="33">
-        <v>0.4.0</v>
+        <v>0.4</v>
       </c>
       <c r="N43" s="33"/>
       <c r="O43" s="33"/>
@@ -3837,7 +3840,7 @@
         <v>11</v>
       </c>
       <c r="M44" s="53">
-        <v>0.02.0</v>
+        <v>0.02</v>
       </c>
       <c r="N44" s="33"/>
       <c r="O44" s="33"/>
@@ -3849,7 +3852,7 @@
       <c r="U44" s="54"/>
       <c r="Z44" s="164"/>
       <c r="AE44" s="41">
-        <v>13.4.0</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="45" spans="1:94" customHeight="1" ht="24.9">
@@ -3868,7 +3871,7 @@
         <v>12</v>
       </c>
       <c r="M45" s="53">
-        <v>0.04.0</v>
+        <v>0.04</v>
       </c>
       <c r="N45" s="33"/>
       <c r="O45" s="33"/>
@@ -3880,7 +3883,7 @@
       <c r="U45" s="54"/>
       <c r="Z45" s="164"/>
       <c r="AE45" s="41">
-        <v>9.4.0</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="46" spans="1:94" customHeight="1" ht="24.9">
@@ -3899,7 +3902,7 @@
         <v>13</v>
       </c>
       <c r="M46" s="53">
-        <v>0.06.0</v>
+        <v>0.06</v>
       </c>
       <c r="N46" s="33"/>
       <c r="O46" s="33"/>
@@ -3927,7 +3930,7 @@
         <v>14</v>
       </c>
       <c r="M47" s="53">
-        <v>0.08.0</v>
+        <v>0.08</v>
       </c>
       <c r="N47" s="33"/>
       <c r="O47" s="33"/>
@@ -3956,7 +3959,7 @@
         <v>15</v>
       </c>
       <c r="M48" s="53">
-        <v>0.02.0</v>
+        <v>0.02</v>
       </c>
       <c r="N48" s="33"/>
       <c r="O48" s="33"/>
@@ -3984,7 +3987,7 @@
         <v>16</v>
       </c>
       <c r="M49" s="33">
-        <v>0.03.0</v>
+        <v>0.03</v>
       </c>
       <c r="N49" s="33"/>
       <c r="O49" s="33"/>
@@ -4011,7 +4014,7 @@
         <v>17</v>
       </c>
       <c r="M50" s="33">
-        <v>0.5.0</v>
+        <v>0.5</v>
       </c>
       <c r="N50" s="129"/>
       <c r="O50" s="129"/>
@@ -4038,7 +4041,7 @@
         <v>18</v>
       </c>
       <c r="M51" s="53">
-        <v>0.5.0</v>
+        <v>0.5</v>
       </c>
       <c r="N51" s="129"/>
       <c r="O51" s="33"/>
@@ -4090,7 +4093,7 @@
         <v>19</v>
       </c>
       <c r="M53" s="33">
-        <v>0.15.0</v>
+        <v>0.15</v>
       </c>
       <c r="N53" s="33"/>
       <c r="O53" s="33"/>
@@ -4124,7 +4127,7 @@
         <v>20</v>
       </c>
       <c r="M54" s="33">
-        <v>0.15.0</v>
+        <v>0.15</v>
       </c>
       <c r="N54" s="129"/>
       <c r="O54" s="33"/>
@@ -4158,7 +4161,7 @@
         <v>21</v>
       </c>
       <c r="M55" s="33">
-        <v>0.3.0</v>
+        <v>0.3</v>
       </c>
       <c r="N55" s="129"/>
       <c r="O55" s="33"/>
@@ -4270,7 +4273,7 @@
         <v>23</v>
       </c>
       <c r="M58" s="42">
-        <v>0.4.0</v>
+        <v>0.4</v>
       </c>
       <c r="N58" s="140"/>
       <c r="O58" s="140"/>
@@ -4299,7 +4302,7 @@
         <v>24</v>
       </c>
       <c r="M59" s="42">
-        <v>0.15.0</v>
+        <v>0.15</v>
       </c>
       <c r="N59" s="142"/>
       <c r="O59" s="142"/>
@@ -4333,7 +4336,7 @@
         <v>25</v>
       </c>
       <c r="M60" s="53">
-        <v>2.5.0</v>
+        <v>2.5</v>
       </c>
       <c r="N60" s="129"/>
       <c r="O60" s="129"/>
@@ -4362,7 +4365,7 @@
         <v>26</v>
       </c>
       <c r="M61" s="33">
-        <v>1.5.0</v>
+        <v>1.5</v>
       </c>
       <c r="N61" s="129"/>
       <c r="O61" s="129"/>
@@ -4658,7 +4661,7 @@
         <v>32</v>
       </c>
       <c r="M71" s="42">
-        <v>2.5.0</v>
+        <v>2.5</v>
       </c>
       <c r="N71" s="142"/>
       <c r="O71" s="142"/>
@@ -4737,7 +4740,7 @@
         <v>34</v>
       </c>
       <c r="M74" s="33">
-        <v>2.5.0</v>
+        <v>2.5</v>
       </c>
       <c r="N74" s="129"/>
       <c r="O74" s="33"/>
@@ -4843,7 +4846,7 @@
         <v>37</v>
       </c>
       <c r="M78" s="33">
-        <v>2.5.0</v>
+        <v>2.5</v>
       </c>
       <c r="N78" s="129"/>
       <c r="O78" s="33"/>
@@ -4934,7 +4937,7 @@
         <v>40</v>
       </c>
       <c r="M81" s="53">
-        <v>0.5.0</v>
+        <v>0.5</v>
       </c>
       <c r="N81" s="129"/>
       <c r="O81" s="129"/>
@@ -5364,7 +5367,7 @@
       <c r="K90" s="261"/>
       <c r="L90" s="173"/>
       <c r="M90" s="72">
-        <v>0.75.0</v>
+        <v>0.75</v>
       </c>
       <c r="N90" s="33"/>
       <c r="O90" s="33"/>
@@ -5467,7 +5470,7 @@
       <c r="K91" s="264"/>
       <c r="L91" s="174"/>
       <c r="M91" s="153">
-        <v>0.25.0</v>
+        <v>0.25</v>
       </c>
       <c r="N91" s="33"/>
       <c r="O91" s="33"/>
@@ -5770,7 +5773,7 @@
       <c r="K94" s="261"/>
       <c r="L94" s="173"/>
       <c r="M94" s="72">
-        <v>1.5.0</v>
+        <v>1.5</v>
       </c>
       <c r="N94" s="33"/>
       <c r="O94" s="33"/>
@@ -7429,7 +7432,7 @@
       <c r="N122" s="37"/>
       <c r="O122" s="37"/>
       <c r="P122" s="243" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="Q122" s="243"/>
       <c r="R122" s="243"/>
@@ -7458,7 +7461,7 @@
       <c r="N123" s="104"/>
       <c r="O123" s="104"/>
       <c r="P123" s="239" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Q123" s="239"/>
       <c r="R123" s="239"/>
@@ -7498,7 +7501,7 @@
     </row>
     <row r="125" spans="1:94" customHeight="1" ht="24.9" s="98" customFormat="1">
       <c r="B125" s="240" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C125" s="241"/>
       <c r="D125" s="241"/>
@@ -7527,7 +7530,7 @@
     <row r="126" spans="1:94" customHeight="1" ht="24.9" s="37" customFormat="1">
       <c r="B126" s="81"/>
       <c r="C126" s="82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D126" s="83"/>
       <c r="E126" s="83"/>
@@ -7555,7 +7558,7 @@
       <c r="A127" s="96"/>
       <c r="B127" s="87"/>
       <c r="C127" s="88" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D127" s="89"/>
       <c r="E127" s="89"/>
@@ -7584,7 +7587,7 @@
       <c r="A128" s="41"/>
       <c r="B128" s="87"/>
       <c r="C128" s="91" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D128" s="92"/>
       <c r="E128" s="92"/>
@@ -7612,7 +7615,7 @@
       <c r="A129" s="41"/>
       <c r="B129" s="87"/>
       <c r="C129" s="91" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D129" s="92"/>
       <c r="E129" s="92"/>
@@ -7650,7 +7653,7 @@
       <c r="L130" s="92"/>
       <c r="M130" s="90"/>
       <c r="O130" s="246" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P130" s="246"/>
       <c r="Q130" s="246"/>
@@ -7676,7 +7679,7 @@
       <c r="L131" s="92"/>
       <c r="M131" s="90"/>
       <c r="O131" s="247" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="P131" s="247"/>
       <c r="Q131" s="247"/>
@@ -7724,7 +7727,7 @@
       <c r="J133" s="92"/>
       <c r="M133" s="90"/>
       <c r="O133" s="243" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="P133" s="247"/>
       <c r="Q133" s="247"/>
@@ -7751,7 +7754,7 @@
       <c r="M134" s="103"/>
       <c r="N134" s="104"/>
       <c r="O134" s="239" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="P134" s="239"/>
       <c r="Q134" s="239"/>
@@ -7836,7 +7839,7 @@
     <row r="138" spans="1:94" customHeight="1" ht="24.9" s="27" customFormat="1">
       <c r="A138" s="7"/>
       <c r="B138" s="240" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C138" s="241"/>
       <c r="D138" s="241"/>
@@ -7866,7 +7869,7 @@
       <c r="A139" s="7"/>
       <c r="B139" s="81"/>
       <c r="C139" s="82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D139" s="83"/>
       <c r="E139" s="83"/>
@@ -7895,7 +7898,7 @@
       <c r="A140" s="7"/>
       <c r="B140" s="87"/>
       <c r="C140" s="88" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D140" s="89"/>
       <c r="E140" s="89"/>
@@ -7910,7 +7913,7 @@
       <c r="N140" s="89"/>
       <c r="O140" s="89"/>
       <c r="P140" s="89" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Q140" s="89"/>
       <c r="R140" s="89"/>
@@ -7926,7 +7929,7 @@
       <c r="A141" s="93"/>
       <c r="B141" s="87"/>
       <c r="C141" s="91" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D141" s="92"/>
       <c r="E141" s="92"/>
@@ -7955,7 +7958,7 @@
       <c r="A142" s="41"/>
       <c r="B142" s="87"/>
       <c r="C142" s="91" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D142" s="92"/>
       <c r="E142" s="92"/>
@@ -8020,7 +8023,7 @@
       <c r="L144" s="92"/>
       <c r="M144" s="90"/>
       <c r="P144" s="243" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="Q144" s="243"/>
       <c r="R144" s="243"/>
@@ -8047,7 +8050,7 @@
       <c r="L145" s="92"/>
       <c r="M145" s="90"/>
       <c r="P145" s="246" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Q145" s="246"/>
       <c r="R145" s="246"/>
@@ -8140,7 +8143,7 @@
       <c r="N149" s="37"/>
       <c r="O149" s="37"/>
       <c r="P149" s="243" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="Q149" s="243"/>
       <c r="R149" s="243"/>
@@ -8163,7 +8166,7 @@
       <c r="N150" s="104"/>
       <c r="O150" s="104"/>
       <c r="P150" s="239" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Q150" s="239"/>
       <c r="R150" s="239"/>
@@ -8193,7 +8196,7 @@
     </row>
     <row r="152" spans="1:94" customHeight="1" ht="24.9">
       <c r="B152" s="240" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C152" s="241"/>
       <c r="D152" s="241"/>
@@ -8217,7 +8220,7 @@
     <row r="153" spans="1:94" customHeight="1" ht="24.9">
       <c r="B153" s="81"/>
       <c r="C153" s="82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D153" s="83"/>
       <c r="E153" s="83"/>
@@ -8240,7 +8243,7 @@
     <row r="154" spans="1:94" customHeight="1" ht="24.9">
       <c r="B154" s="87"/>
       <c r="C154" s="88" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D154" s="89"/>
       <c r="E154" s="89"/>
@@ -8255,7 +8258,7 @@
       <c r="N154" s="89"/>
       <c r="O154" s="89"/>
       <c r="P154" s="89" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Q154" s="89"/>
       <c r="R154" s="89"/>
@@ -8265,7 +8268,7 @@
     <row r="155" spans="1:94" customHeight="1" ht="24.9">
       <c r="B155" s="87"/>
       <c r="C155" s="91" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D155" s="92"/>
       <c r="E155" s="92"/>
@@ -8288,7 +8291,7 @@
     <row r="156" spans="1:94" customHeight="1" ht="24.9" s="37" customFormat="1">
       <c r="B156" s="87"/>
       <c r="C156" s="91" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D156" s="92"/>
       <c r="E156" s="92"/>
@@ -8328,7 +8331,7 @@
       <c r="N157" s="92"/>
       <c r="O157" s="92"/>
       <c r="P157" s="92" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Q157" s="92"/>
       <c r="R157" s="92"/>
@@ -8380,7 +8383,7 @@
       <c r="N159" s="92"/>
       <c r="O159" s="92"/>
       <c r="P159" s="101" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Q159" s="101"/>
       <c r="R159" s="101"/>
@@ -8407,7 +8410,7 @@
       <c r="N160" s="101"/>
       <c r="O160" s="101"/>
       <c r="P160" s="101" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q160" s="101"/>
       <c r="R160" s="101"/>

</xml_diff>